<commit_message>
changes code to update folder structure code
</commit_message>
<xml_diff>
--- a/content_extraction/Mapped.xlsx
+++ b/content_extraction/Mapped.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nitin\Desktop\projects\my-app\content_extraction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A003548-C2C4-4F03-B2DA-4E0D9D5668FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B05753E9-618E-4F4C-8DA8-0A1EAF1BF178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -195,18 +195,6 @@
     <t>ParkDetails/InAroundPark/Components/IntroductionComponent/SecondColumnText</t>
   </si>
   <si>
-    <t>ParkDetails/InAroundPark/Components/ContentBlockComponent/Title</t>
-  </si>
-  <si>
-    <t>ParkDetails/InAroundPark/Components/ContentBlockComponent/Text</t>
-  </si>
-  <si>
-    <t>ParkDetails/InAroundPark/Components/ContentBlockComponent/ImageContentid</t>
-  </si>
-  <si>
-    <t>ParkDetails/InAroundPark/Components/ContentBlockComponent/ImageAltText</t>
-  </si>
-  <si>
     <t>ParkDetails/SurroundingParks/Components/SurroundingMainVisualWithOfferLabel/Title</t>
   </si>
   <si>
@@ -255,9 +243,6 @@
     <t>ParkDetails/AccomodationList</t>
   </si>
   <si>
-    <t>ParkDetails/InAroundPark/Components/ContentBlockComponent</t>
-  </si>
-  <si>
     <t>ParkDetails/InAroundPark/Components/ParkHomeImageAccordionComponent/AccordionList</t>
   </si>
   <si>
@@ -274,6 +259,21 @@
   </si>
   <si>
     <t>ParkDetails/Components/ParkHomeImageAccordionComponent/AccordionList</t>
+  </si>
+  <si>
+    <t>ParkDetails/InAroundPark/Components/ContentBlockComponent/Blocks</t>
+  </si>
+  <si>
+    <t>ParkDetails/InAroundPark/Components/ContentBlockComponent/Blocks/Title</t>
+  </si>
+  <si>
+    <t>ParkDetails/InAroundPark/Components/ContentBlockComponent/Blocks/Text</t>
+  </si>
+  <si>
+    <t>ParkDetails/InAroundPark/Components/ContentBlockComponent/Blocks/ImageContentid</t>
+  </si>
+  <si>
+    <t>ParkDetails/InAroundPark/Components/ContentBlockComponent/Blocks/ImageAltText</t>
   </si>
 </sst>
 </file>
@@ -672,8 +672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -692,10 +692,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
@@ -864,7 +864,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B15" t="s">
         <v>3</v>
@@ -919,7 +919,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B20" t="s">
         <v>3</v>
@@ -974,7 +974,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B25" t="s">
         <v>3</v>
@@ -1040,7 +1040,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B31" t="s">
         <v>3</v>
@@ -1084,7 +1084,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D35" t="s">
         <v>25</v>
@@ -1180,7 +1180,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" s="4" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B44" t="s">
         <v>3</v>
@@ -1268,7 +1268,7 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" s="5" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B52" t="s">
         <v>3</v>
@@ -1279,7 +1279,7 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" s="5" t="s">
-        <v>56</v>
+        <v>79</v>
       </c>
       <c r="B53" t="s">
         <v>3</v>
@@ -1290,7 +1290,7 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" s="4" t="s">
-        <v>57</v>
+        <v>80</v>
       </c>
       <c r="B54" t="s">
         <v>3</v>
@@ -1301,7 +1301,7 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="B55" t="s">
         <v>3</v>
@@ -1312,7 +1312,7 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" s="5" t="s">
-        <v>59</v>
+        <v>82</v>
       </c>
       <c r="B56" t="s">
         <v>3</v>
@@ -1323,7 +1323,7 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" s="5" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B57" t="s">
         <v>3</v>
@@ -1334,7 +1334,7 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" s="5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B58" t="s">
         <v>3</v>
@@ -1345,7 +1345,7 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" s="5" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B59" t="s">
         <v>3</v>
@@ -1356,7 +1356,7 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" s="5" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B60" t="s">
         <v>3</v>
@@ -1367,7 +1367,7 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" s="5" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B61" t="s">
         <v>3</v>
@@ -1378,7 +1378,7 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" s="5" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B62" t="s">
         <v>3</v>
@@ -1389,10 +1389,10 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B63" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D63" t="s">
         <v>25</v>
@@ -1400,13 +1400,13 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" s="2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C64" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D64" t="s">
         <v>4</v>
@@ -1414,13 +1414,13 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" s="2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C65" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D65" t="s">
         <v>4</v>
@@ -1428,13 +1428,13 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B66" t="s">
         <v>70</v>
       </c>
-      <c r="B66" t="s">
-        <v>74</v>
-      </c>
       <c r="C66" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D66" t="s">
         <v>4</v>
@@ -1442,13 +1442,13 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" s="2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B67" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C67" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D67" t="s">
         <v>4</v>

</xml_diff>